<commit_message>
Replace "DeviceSettings" with "Device.Settings" in various files
 * Replaced "DeviceSettings" with "Device.Settings" in various files.
  - Removed EgsDeviceSettings DeviceSettings from EgsHostOnUserControl.
  - Set [Obsolete] attribute to EgsDevice.SetSettings(EgsDeviceSettings settings) and EgsDevice.GetDefaultEgsDevice(EgsDeviceSettings settings).
 * Updated SDK dll files and example programs.
  - Removed "EgsDeviceSettings Settings { get; set; }".
  - Fixed various bugs.
</commit_message>
<xml_diff>
--- a/Documents/UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx
+++ b/Documents/UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1579" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="636">
   <si>
     <t>MessageId</t>
   </si>
@@ -2624,10 +2624,6 @@
   </si>
   <si>
     <t>public</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>internal</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -6333,10 +6329,10 @@
   <dimension ref="A1:AD64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6352,10 +6348,10 @@
     <col min="9" max="9" width="3.75" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.5" style="2" customWidth="1"/>
     <col min="11" max="11" width="6.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" style="2" customWidth="1"/>
+    <col min="13" max="13" width="19.125" style="2" customWidth="1"/>
     <col min="14" max="19" width="10.625" style="2" customWidth="1"/>
-    <col min="20" max="21" width="7.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="7.375" style="2" customWidth="1"/>
     <col min="22" max="22" width="8.25" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="21.875" style="2" bestFit="1" customWidth="1"/>
@@ -6436,7 +6432,7 @@
         <v>349</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>171</v>
@@ -6522,7 +6518,7 @@
         <v>342</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>131</v>
@@ -6534,7 +6530,7 @@
         <v>370</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -6608,7 +6604,7 @@
         <v>371</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -6682,7 +6678,7 @@
         <v>414</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -6759,7 +6755,7 @@
         <v>372</v>
       </c>
       <c r="AC5" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="85.5">
@@ -6842,10 +6838,10 @@
         <v>471</v>
       </c>
       <c r="AC6" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="AD6" s="4" t="s">
         <v>577</v>
-      </c>
-      <c r="AD6" s="4" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -6930,10 +6926,10 @@
         <v>277</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>177</v>
@@ -6945,7 +6941,7 @@
         <v>42</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>69</v>
@@ -6963,10 +6959,10 @@
         <v>236</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="W8" s="2" t="s">
         <v>325</v>
@@ -6975,13 +6971,13 @@
         <v>113</v>
       </c>
       <c r="Y8" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="AA8" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="AA8" s="1" t="s">
-        <v>547</v>
-      </c>
       <c r="AC8" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -7046,7 +7042,7 @@
         <v>337</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>342</v>
+        <v>32</v>
       </c>
       <c r="W9" s="2" t="s">
         <v>325</v>
@@ -7058,7 +7054,7 @@
         <v>375</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -7123,7 +7119,7 @@
         <v>338</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>342</v>
+        <v>32</v>
       </c>
       <c r="W10" s="2" t="s">
         <v>325</v>
@@ -7135,7 +7131,7 @@
         <v>376</v>
       </c>
       <c r="AC10" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="57">
@@ -7218,10 +7214,10 @@
         <v>450</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="28.5">
@@ -7289,7 +7285,7 @@
         <v>344</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="X12" s="2" t="s">
         <v>121</v>
@@ -7307,7 +7303,7 @@
         <v>62</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="AD12" s="4" t="s">
         <v>433</v>
@@ -7396,10 +7392,10 @@
         <v>434</v>
       </c>
       <c r="AC13" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="AD13" s="4" t="s">
         <v>580</v>
-      </c>
-      <c r="AD13" s="4" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="57">
@@ -7485,10 +7481,10 @@
         <v>435</v>
       </c>
       <c r="AC14" s="4" t="s">
+        <v>620</v>
+      </c>
+      <c r="AD14" s="4" t="s">
         <v>621</v>
-      </c>
-      <c r="AD14" s="4" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="28.5">
@@ -7565,10 +7561,10 @@
         <v>419</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AD15" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -7576,17 +7572,20 @@
         <v>277</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="K16" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="L16" s="2" t="s">
         <v>69</v>
       </c>
@@ -7621,7 +7620,7 @@
         <v>379</v>
       </c>
       <c r="AC16" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="71.25">
@@ -7629,17 +7628,20 @@
         <v>277</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="K17" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="L17" s="2" t="s">
         <v>69</v>
       </c>
@@ -7665,22 +7667,22 @@
         <v>197</v>
       </c>
       <c r="Y17" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="AA17" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="Z17" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="AA17" s="1" t="s">
+      <c r="AB17" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="AB17" s="1" t="s">
-        <v>551</v>
-      </c>
       <c r="AC17" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="28.5">
@@ -7688,10 +7690,10 @@
         <v>277</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>22</v>
@@ -7712,10 +7714,10 @@
         <v>85</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>69</v>
@@ -7745,22 +7747,22 @@
         <v>336</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="42.75">
@@ -7768,10 +7770,10 @@
         <v>277</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>85</v>
@@ -7779,6 +7781,9 @@
       <c r="J19" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="K19" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="L19" s="2" t="s">
         <v>69</v>
       </c>
@@ -7807,13 +7812,13 @@
         <v>111</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="AA19" s="1" t="s">
         <v>380</v>
       </c>
       <c r="AC19" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="20" spans="1:30" ht="28.5">
@@ -7821,10 +7826,10 @@
         <v>277</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>22</v>
@@ -7845,10 +7850,10 @@
         <v>85</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>69</v>
@@ -7878,22 +7883,22 @@
         <v>338</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Y20" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="AA20" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="AA20" s="1" t="s">
-        <v>565</v>
-      </c>
       <c r="AC20" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="21" spans="1:30">
@@ -7973,7 +7978,7 @@
         <v>381</v>
       </c>
       <c r="AC21" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="42.75">
@@ -8053,7 +8058,7 @@
         <v>382</v>
       </c>
       <c r="AC22" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="23" spans="1:30">
@@ -8133,7 +8138,7 @@
         <v>383</v>
       </c>
       <c r="AC23" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="24" spans="1:30" ht="28.5">
@@ -8186,7 +8191,7 @@
         <v>474</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="X24" s="2" t="s">
         <v>124</v>
@@ -8204,10 +8209,10 @@
         <v>423</v>
       </c>
       <c r="AC24" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="AD24" s="4" t="s">
         <v>588</v>
-      </c>
-      <c r="AD24" s="4" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="42.75">
@@ -8275,7 +8280,7 @@
         <v>32</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="X25" s="2" t="s">
         <v>110</v>
@@ -8287,7 +8292,7 @@
         <v>384</v>
       </c>
       <c r="AC25" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="57">
@@ -8373,7 +8378,7 @@
         <v>439</v>
       </c>
       <c r="AD26" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="27" spans="1:30" ht="28.5">
@@ -8435,7 +8440,7 @@
         <v>344</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Y27" s="1" t="s">
         <v>141</v>
@@ -8444,7 +8449,7 @@
         <v>385</v>
       </c>
       <c r="AC27" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="28" spans="1:30" ht="42.75">
@@ -8527,10 +8532,10 @@
         <v>426</v>
       </c>
       <c r="AC28" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="AD28" s="4" t="s">
         <v>592</v>
-      </c>
-      <c r="AD28" s="4" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="57">
@@ -8613,7 +8618,7 @@
         <v>440</v>
       </c>
       <c r="AD29" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="30" spans="1:30">
@@ -8678,7 +8683,7 @@
         <v>387</v>
       </c>
       <c r="AC30" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="31" spans="1:30" ht="28.5">
@@ -8829,7 +8834,7 @@
         <v>389</v>
       </c>
       <c r="AC32" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="33" spans="1:30" ht="28.5">
@@ -8977,7 +8982,7 @@
         <v>391</v>
       </c>
       <c r="AC34" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="35" spans="1:30" ht="42.75">
@@ -9060,7 +9065,7 @@
         <v>350</v>
       </c>
       <c r="AC35" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="AD35" s="4" t="s">
         <v>443</v>
@@ -9074,7 +9079,7 @@
         <v>289</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>22</v>
@@ -9134,13 +9139,13 @@
         <v>198</v>
       </c>
       <c r="Y36" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="AA36" s="1" t="s">
         <v>393</v>
       </c>
       <c r="AC36" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="37" spans="1:30" ht="28.5">
@@ -9217,7 +9222,7 @@
         <v>394</v>
       </c>
       <c r="AC37" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="38" spans="1:30" ht="28.5">
@@ -9279,7 +9284,7 @@
         <v>200</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X38" s="2" t="s">
         <v>113</v>
@@ -9291,7 +9296,7 @@
         <v>395</v>
       </c>
       <c r="AC38" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="39" spans="1:30" ht="28.5">
@@ -9353,7 +9358,7 @@
         <v>200</v>
       </c>
       <c r="W39" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X39" s="2" t="s">
         <v>516</v>
@@ -9365,7 +9370,7 @@
         <v>396</v>
       </c>
       <c r="AC39" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="40" spans="1:30" ht="57">
@@ -9421,7 +9426,7 @@
         <v>200</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X40" s="2" t="s">
         <v>489</v>
@@ -9433,7 +9438,7 @@
         <v>397</v>
       </c>
       <c r="AC40" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="41" spans="1:30" ht="114">
@@ -9516,10 +9521,10 @@
         <v>436</v>
       </c>
       <c r="AC41" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AD41" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="42" spans="1:30" ht="28.5">
@@ -9554,13 +9559,13 @@
         <v>68</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>528</v>
+        <v>33</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>117</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="O42" s="2" t="s">
         <v>478</v>
@@ -9581,7 +9586,7 @@
         <v>200</v>
       </c>
       <c r="W42" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X42" s="2" t="s">
         <v>113</v>
@@ -9593,7 +9598,7 @@
         <v>399</v>
       </c>
       <c r="AC42" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="43" spans="1:30" ht="28.5">
@@ -9655,7 +9660,7 @@
         <v>200</v>
       </c>
       <c r="W43" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X43" s="2" t="s">
         <v>517</v>
@@ -9667,7 +9672,7 @@
         <v>503</v>
       </c>
       <c r="AC43" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="44" spans="1:30" ht="42.75">
@@ -9729,7 +9734,7 @@
         <v>200</v>
       </c>
       <c r="W44" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X44" s="2" t="s">
         <v>512</v>
@@ -9741,7 +9746,7 @@
         <v>400</v>
       </c>
       <c r="AC44" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="45" spans="1:30" ht="28.5">
@@ -9803,7 +9808,7 @@
         <v>200</v>
       </c>
       <c r="W45" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X45" s="2" t="s">
         <v>518</v>
@@ -9815,7 +9820,7 @@
         <v>504</v>
       </c>
       <c r="AC45" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="46" spans="1:30" ht="42.75">
@@ -9877,7 +9882,7 @@
         <v>200</v>
       </c>
       <c r="W46" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X46" s="2" t="s">
         <v>511</v>
@@ -9889,7 +9894,7 @@
         <v>401</v>
       </c>
       <c r="AC46" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="47" spans="1:30" ht="28.5">
@@ -9945,7 +9950,7 @@
         <v>200</v>
       </c>
       <c r="W47" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="Y47" s="1" t="s">
         <v>484</v>
@@ -9954,7 +9959,7 @@
         <v>485</v>
       </c>
       <c r="AC47" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="48" spans="1:30" ht="28.5">
@@ -10010,7 +10015,7 @@
         <v>32</v>
       </c>
       <c r="W48" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X48" s="2" t="s">
         <v>113</v>
@@ -10022,7 +10027,7 @@
         <v>505</v>
       </c>
       <c r="AC48" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="49" spans="1:30" ht="28.5">
@@ -10078,7 +10083,7 @@
         <v>32</v>
       </c>
       <c r="W49" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X49" s="2" t="s">
         <v>519</v>
@@ -10090,7 +10095,7 @@
         <v>506</v>
       </c>
       <c r="AC49" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="50" spans="1:30" ht="28.5">
@@ -10146,7 +10151,7 @@
         <v>32</v>
       </c>
       <c r="W50" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X50" s="2" t="s">
         <v>520</v>
@@ -10158,7 +10163,7 @@
         <v>507</v>
       </c>
       <c r="AC50" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="51" spans="1:30" ht="28.5">
@@ -10223,7 +10228,7 @@
         <v>200</v>
       </c>
       <c r="W51" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X51" s="2" t="s">
         <v>113</v>
@@ -10235,7 +10240,7 @@
         <v>508</v>
       </c>
       <c r="AC51" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="52" spans="1:30" ht="28.5">
@@ -10300,7 +10305,7 @@
         <v>200</v>
       </c>
       <c r="W52" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X52" s="2" t="s">
         <v>521</v>
@@ -10312,7 +10317,7 @@
         <v>509</v>
       </c>
       <c r="AC52" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="53" spans="1:30" ht="28.5">
@@ -10377,7 +10382,7 @@
         <v>200</v>
       </c>
       <c r="W53" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="X53" s="2" t="s">
         <v>522</v>
@@ -10389,7 +10394,7 @@
         <v>510</v>
       </c>
       <c r="AC53" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="54" spans="1:30" ht="171">
@@ -10472,10 +10477,10 @@
         <v>452</v>
       </c>
       <c r="AC54" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AD54" s="5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="55" spans="1:30" ht="28.5">
@@ -10558,7 +10563,7 @@
         <v>469</v>
       </c>
       <c r="AC55" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="AD55" s="4" t="s">
         <v>481</v>
@@ -10635,7 +10640,7 @@
         <v>403</v>
       </c>
       <c r="AC56" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="57" spans="1:30">
@@ -10709,7 +10714,7 @@
         <v>404</v>
       </c>
       <c r="AC57" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="58" spans="1:30">
@@ -10783,7 +10788,7 @@
         <v>405</v>
       </c>
       <c r="AC58" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="59" spans="1:30">
@@ -10857,7 +10862,7 @@
         <v>406</v>
       </c>
       <c r="AC59" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="60" spans="1:30">
@@ -10931,7 +10936,7 @@
         <v>407</v>
       </c>
       <c r="AC60" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="61" spans="1:30">
@@ -11005,7 +11010,7 @@
         <v>408</v>
       </c>
       <c r="AC61" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="62" spans="1:30" ht="28.5">
@@ -11067,7 +11072,7 @@
         <v>354</v>
       </c>
       <c r="W62" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="X62" s="2" t="s">
         <v>172</v>
@@ -11079,7 +11084,7 @@
         <v>409</v>
       </c>
       <c r="AC62" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="63" spans="1:30" ht="28.5">
@@ -11144,7 +11149,7 @@
         <v>344</v>
       </c>
       <c r="W63" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="Y63" s="1" t="s">
         <v>135</v>
@@ -11153,7 +11158,7 @@
         <v>410</v>
       </c>
       <c r="AC63" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="64" spans="1:30">
@@ -11230,7 +11235,7 @@
         <v>463</v>
       </c>
       <c r="AC64" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bugs caused by DataBinding and so on
</commit_message>
<xml_diff>
--- a/Documents/UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx
+++ b/Documents/UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx
@@ -2757,10 +2757,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>EnumValueWithDescription&lt;FaceDetectionMethodKind&gt;</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="8"/>
@@ -5327,6 +5323,10 @@
   </si>
   <si>
     <t>false</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>FaceDetectionMethodOptions</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -6329,10 +6329,10 @@
   <dimension ref="A1:AD64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6530,7 +6530,7 @@
         <v>370</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -6604,7 +6604,7 @@
         <v>371</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -6678,7 +6678,7 @@
         <v>414</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -6755,7 +6755,7 @@
         <v>372</v>
       </c>
       <c r="AC5" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="85.5">
@@ -6838,10 +6838,10 @@
         <v>471</v>
       </c>
       <c r="AC6" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="AD6" s="4" t="s">
         <v>576</v>
-      </c>
-      <c r="AD6" s="4" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -6977,7 +6977,7 @@
         <v>546</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -7054,7 +7054,7 @@
         <v>375</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -7131,7 +7131,7 @@
         <v>376</v>
       </c>
       <c r="AC10" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="57">
@@ -7214,10 +7214,10 @@
         <v>450</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="28.5">
@@ -7303,7 +7303,7 @@
         <v>62</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AD12" s="4" t="s">
         <v>433</v>
@@ -7392,10 +7392,10 @@
         <v>434</v>
       </c>
       <c r="AC13" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="AD13" s="4" t="s">
         <v>579</v>
-      </c>
-      <c r="AD13" s="4" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="57">
@@ -7481,10 +7481,10 @@
         <v>435</v>
       </c>
       <c r="AC14" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="AD14" s="4" t="s">
         <v>620</v>
-      </c>
-      <c r="AD14" s="4" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="28.5">
@@ -7561,10 +7561,10 @@
         <v>419</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="AD15" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -7620,7 +7620,7 @@
         <v>379</v>
       </c>
       <c r="AC16" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="71.25">
@@ -7628,7 +7628,7 @@
         <v>277</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>554</v>
+        <v>635</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>547</v>
@@ -7679,10 +7679,10 @@
         <v>550</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="28.5">
@@ -7756,13 +7756,13 @@
         <v>542</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="42.75">
@@ -7773,7 +7773,7 @@
         <v>540</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>85</v>
@@ -7812,13 +7812,13 @@
         <v>111</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="AA19" s="1" t="s">
         <v>380</v>
       </c>
       <c r="AC19" s="6" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="20" spans="1:30" ht="28.5">
@@ -7829,7 +7829,7 @@
         <v>539</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>22</v>
@@ -7850,7 +7850,7 @@
         <v>85</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>32</v>
@@ -7889,16 +7889,16 @@
         <v>531</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="Y20" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="AA20" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="AA20" s="1" t="s">
-        <v>564</v>
-      </c>
       <c r="AC20" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="21" spans="1:30">
@@ -7978,7 +7978,7 @@
         <v>381</v>
       </c>
       <c r="AC21" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="42.75">
@@ -8058,7 +8058,7 @@
         <v>382</v>
       </c>
       <c r="AC22" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="23" spans="1:30">
@@ -8138,7 +8138,7 @@
         <v>383</v>
       </c>
       <c r="AC23" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="24" spans="1:30" ht="28.5">
@@ -8209,10 +8209,10 @@
         <v>423</v>
       </c>
       <c r="AC24" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="AD24" s="4" t="s">
         <v>587</v>
-      </c>
-      <c r="AD24" s="4" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="42.75">
@@ -8292,7 +8292,7 @@
         <v>384</v>
       </c>
       <c r="AC25" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="57">
@@ -8378,7 +8378,7 @@
         <v>439</v>
       </c>
       <c r="AD26" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="27" spans="1:30" ht="28.5">
@@ -8449,7 +8449,7 @@
         <v>385</v>
       </c>
       <c r="AC27" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="28" spans="1:30" ht="42.75">
@@ -8532,10 +8532,10 @@
         <v>426</v>
       </c>
       <c r="AC28" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="AD28" s="4" t="s">
         <v>591</v>
-      </c>
-      <c r="AD28" s="4" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="57">
@@ -8618,7 +8618,7 @@
         <v>440</v>
       </c>
       <c r="AD29" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="30" spans="1:30">
@@ -8683,7 +8683,7 @@
         <v>387</v>
       </c>
       <c r="AC30" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="31" spans="1:30" ht="28.5">
@@ -8834,7 +8834,7 @@
         <v>389</v>
       </c>
       <c r="AC32" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="33" spans="1:30" ht="28.5">
@@ -8982,7 +8982,7 @@
         <v>391</v>
       </c>
       <c r="AC34" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="35" spans="1:30" ht="42.75">
@@ -9065,7 +9065,7 @@
         <v>350</v>
       </c>
       <c r="AC35" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="AD35" s="4" t="s">
         <v>443</v>
@@ -9079,7 +9079,7 @@
         <v>289</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>22</v>
@@ -9139,13 +9139,13 @@
         <v>198</v>
       </c>
       <c r="Y36" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AA36" s="1" t="s">
         <v>393</v>
       </c>
       <c r="AC36" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="37" spans="1:30" ht="28.5">
@@ -9222,7 +9222,7 @@
         <v>394</v>
       </c>
       <c r="AC37" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="38" spans="1:30" ht="28.5">
@@ -9296,7 +9296,7 @@
         <v>395</v>
       </c>
       <c r="AC38" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="39" spans="1:30" ht="28.5">
@@ -9370,7 +9370,7 @@
         <v>396</v>
       </c>
       <c r="AC39" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="40" spans="1:30" ht="57">
@@ -9438,7 +9438,7 @@
         <v>397</v>
       </c>
       <c r="AC40" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="41" spans="1:30" ht="114">
@@ -9521,10 +9521,10 @@
         <v>436</v>
       </c>
       <c r="AC41" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="AD41" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="42" spans="1:30" ht="28.5">
@@ -9598,7 +9598,7 @@
         <v>399</v>
       </c>
       <c r="AC42" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="43" spans="1:30" ht="28.5">
@@ -9672,7 +9672,7 @@
         <v>503</v>
       </c>
       <c r="AC43" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="44" spans="1:30" ht="42.75">
@@ -9746,7 +9746,7 @@
         <v>400</v>
       </c>
       <c r="AC44" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="45" spans="1:30" ht="28.5">
@@ -9820,7 +9820,7 @@
         <v>504</v>
       </c>
       <c r="AC45" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="46" spans="1:30" ht="42.75">
@@ -9894,7 +9894,7 @@
         <v>401</v>
       </c>
       <c r="AC46" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="47" spans="1:30" ht="28.5">
@@ -9959,7 +9959,7 @@
         <v>485</v>
       </c>
       <c r="AC47" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="48" spans="1:30" ht="28.5">
@@ -10027,7 +10027,7 @@
         <v>505</v>
       </c>
       <c r="AC48" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="49" spans="1:30" ht="28.5">
@@ -10095,7 +10095,7 @@
         <v>506</v>
       </c>
       <c r="AC49" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="50" spans="1:30" ht="28.5">
@@ -10163,7 +10163,7 @@
         <v>507</v>
       </c>
       <c r="AC50" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="51" spans="1:30" ht="28.5">
@@ -10240,7 +10240,7 @@
         <v>508</v>
       </c>
       <c r="AC51" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="52" spans="1:30" ht="28.5">
@@ -10317,7 +10317,7 @@
         <v>509</v>
       </c>
       <c r="AC52" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="53" spans="1:30" ht="28.5">
@@ -10394,7 +10394,7 @@
         <v>510</v>
       </c>
       <c r="AC53" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="54" spans="1:30" ht="171">
@@ -10477,10 +10477,10 @@
         <v>452</v>
       </c>
       <c r="AC54" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AD54" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="55" spans="1:30" ht="28.5">
@@ -10563,7 +10563,7 @@
         <v>469</v>
       </c>
       <c r="AC55" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="AD55" s="4" t="s">
         <v>481</v>
@@ -10640,7 +10640,7 @@
         <v>403</v>
       </c>
       <c r="AC56" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="57" spans="1:30">
@@ -10714,7 +10714,7 @@
         <v>404</v>
       </c>
       <c r="AC57" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="58" spans="1:30">
@@ -10788,7 +10788,7 @@
         <v>405</v>
       </c>
       <c r="AC58" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="59" spans="1:30">
@@ -10862,7 +10862,7 @@
         <v>406</v>
       </c>
       <c r="AC59" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="60" spans="1:30">
@@ -10936,7 +10936,7 @@
         <v>407</v>
       </c>
       <c r="AC60" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="61" spans="1:30">
@@ -11010,7 +11010,7 @@
         <v>408</v>
       </c>
       <c r="AC61" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="62" spans="1:30" ht="28.5">
@@ -11084,7 +11084,7 @@
         <v>409</v>
       </c>
       <c r="AC62" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="63" spans="1:30" ht="28.5">
@@ -11158,7 +11158,7 @@
         <v>410</v>
       </c>
       <c r="AC63" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="64" spans="1:30">
@@ -11235,7 +11235,7 @@
         <v>463</v>
       </c>
       <c r="AC64" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
   </sheetData>
@@ -11251,20 +11251,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11427,6 +11427,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FB82232-58B1-4A1D-8A4E-B5C95C1862BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153E850E-4F75-454A-AFBA-A711FED549FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -11439,14 +11447,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FB82232-58B1-4A1D-8A4E-B5C95C1862BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update resource files and source code about "Device Usage" property
</commit_message>
<xml_diff>
--- a/Documents/UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx
+++ b/Documents/UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="638">
   <si>
     <t>MessageId</t>
   </si>
@@ -750,11 +750,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>0:Gesture Camera
-1:Web Camera</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>Basic</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -1936,11 +1931,6 @@
   </si>
   <si>
     <t>固件版本</t>
-  </si>
-  <si>
-    <t>0:ジェスチャーカメラ
-1:ウェブカメラ</t>
-    <phoneticPr fontId="18"/>
   </si>
   <si>
     <t>0:MultiTouch
@@ -3011,79 +3001,6 @@
   </si>
   <si>
     <r>
-      <t>0:手</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t>势摄</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>像</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">头
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>1:网</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t>络摄</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>像</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t>头</t>
-    </r>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <r>
       <t>由</t>
     </r>
     <r>
@@ -5195,20 +5112,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <r>
-      <t>用途</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t>选项</t>
-    </r>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>ZkooTutorial changes the value.  Developer can change it, too.</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -5327,6 +5230,153 @@
       </rPr>
       <t>解决方案</t>
     </r>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>0:Remote Touch
+2:Motion Control
+1:Web Camera</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>0:リモートタッチ
+2:モーションコントロール
+1:ウェブカメラ</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <r>
+      <t>模式</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="FangSong"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>选择</t>
+    </r>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <r>
+      <t>0:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+      </rPr>
+      <t>远</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>程触控</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+      </rPr>
+      <t>动</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>作控制</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>1:网</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+      </rPr>
+      <t>络摄</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>像</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+      </rPr>
+      <t>头</t>
+    </r>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1.1.9000</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>public</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -6329,10 +6379,10 @@
   <dimension ref="A1:AD64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="X16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD29" sqref="AD29"/>
+      <selection pane="bottomRight" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -6366,7 +6416,7 @@
   <sheetData>
     <row r="1" spans="1:30" ht="57" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>75</v>
@@ -6396,16 +6446,16 @@
         <v>34</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>116</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>67</v>
@@ -6423,45 +6473,45 @@
         <v>161</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>166</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>359</v>
-      </c>
       <c r="AA1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="AD1" s="4" t="s">
         <v>401</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>427</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>124</v>
@@ -6494,7 +6544,7 @@
         <v>125</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>36</v>
@@ -6509,16 +6559,16 @@
         <v>163</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>126</v>
@@ -6527,33 +6577,33 @@
         <v>132</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>340</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>99</v>
@@ -6571,16 +6621,16 @@
         <v>42</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>36</v>
@@ -6589,45 +6639,45 @@
         <v>36</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>127</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>340</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>98</v>
@@ -6645,16 +6695,16 @@
         <v>42</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>36</v>
@@ -6663,33 +6713,33 @@
         <v>36</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>128</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>22</v>
@@ -6707,7 +6757,7 @@
         <v>77</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>69</v>
@@ -6719,7 +6769,7 @@
         <v>42</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>163</v>
@@ -6728,7 +6778,7 @@
         <v>36</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>36</v>
@@ -6737,36 +6787,36 @@
         <v>36</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AC5" s="4" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>22</v>
@@ -6778,10 +6828,10 @@
         <v>23</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>85</v>
@@ -6796,10 +6846,10 @@
         <v>42</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>36</v>
@@ -6814,42 +6864,42 @@
         <v>36</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="AC6" s="4" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="AD6" s="4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -6867,10 +6917,10 @@
         <v>107</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>69</v>
@@ -6882,7 +6932,7 @@
         <v>118</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>163</v>
@@ -6900,36 +6950,36 @@
         <v>36</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>129</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>172</v>
@@ -6947,7 +6997,7 @@
         <v>69</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>36</v>
@@ -6956,39 +7006,39 @@
         <v>36</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="V8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="X8" s="2" t="s">
         <v>113</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>22</v>
@@ -7000,7 +7050,7 @@
         <v>26</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>158</v>
@@ -7018,7 +7068,7 @@
         <v>42</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>163</v>
@@ -7036,36 +7086,36 @@
         <v>36</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="V9" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>22</v>
@@ -7077,7 +7127,7 @@
         <v>26</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>158</v>
@@ -7095,7 +7145,7 @@
         <v>42</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>163</v>
@@ -7113,36 +7163,36 @@
         <v>36</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="V10" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Y10" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AC10" s="4" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="57" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>22</v>
@@ -7154,7 +7204,7 @@
         <v>23</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>77</v>
@@ -7172,7 +7222,7 @@
         <v>69</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>36</v>
@@ -7187,45 +7237,45 @@
         <v>163</v>
       </c>
       <c r="T11" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="Z11" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="U11" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="V11" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="W11" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="X11" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="Y11" s="1" t="s">
+      <c r="AA11" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="Z11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="AA11" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>439</v>
-      </c>
       <c r="AC11" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>81</v>
@@ -7264,31 +7314,31 @@
         <v>36</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P12" s="2" t="s">
         <v>36</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="Y12" s="1" t="s">
         <v>131</v>
@@ -7297,24 +7347,24 @@
         <v>62</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AB12" s="1" t="s">
         <v>62</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="AD12" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="57" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
@@ -7347,7 +7397,7 @@
         <v>117</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>36</v>
@@ -7365,45 +7415,45 @@
         <v>36</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W13" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="Y13" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="X13" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="Z13" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="AC13" s="4" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="AD13" s="4" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="57" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>82</v>
@@ -7436,13 +7486,13 @@
         <v>164</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>36</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>36</v>
@@ -7454,45 +7504,45 @@
         <v>36</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="AC14" s="4" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="AD14" s="4" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>185</v>
@@ -7507,7 +7557,7 @@
         <v>23</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>77</v>
@@ -7525,7 +7575,7 @@
         <v>69</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>36</v>
@@ -7537,48 +7587,51 @@
         <v>36</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>461</v>
+        <v>636</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>637</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>186</v>
+        <v>632</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>408</v>
+        <v>633</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="AD15" s="4" t="s">
-        <v>565</v>
+        <v>635</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>42</v>
@@ -7590,7 +7643,7 @@
         <v>69</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>36</v>
@@ -7599,42 +7652,42 @@
         <v>36</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V16" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X16" s="2" t="s">
         <v>111</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AC16" s="4" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>42</v>
@@ -7646,7 +7699,7 @@
         <v>69</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>36</v>
@@ -7655,45 +7708,45 @@
         <v>36</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V17" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>22</v>
@@ -7714,7 +7767,7 @@
         <v>85</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>32</v>
@@ -7723,7 +7776,7 @@
         <v>69</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>36</v>
@@ -7741,39 +7794,39 @@
         <v>36</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="V18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="Y18" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="AA18" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="AA18" s="1" t="s">
-        <v>543</v>
-      </c>
       <c r="AC18" s="1" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>85</v>
@@ -7788,7 +7841,7 @@
         <v>69</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>36</v>
@@ -7797,39 +7850,39 @@
         <v>36</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V19" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X19" s="2" t="s">
         <v>111</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AC19" s="6" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="20" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>22</v>
@@ -7841,7 +7894,7 @@
         <v>23</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>172</v>
@@ -7850,7 +7903,7 @@
         <v>85</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>32</v>
@@ -7859,54 +7912,54 @@
         <v>69</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>36</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="P20" s="2" t="s">
         <v>36</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="V20" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
@@ -7939,7 +7992,7 @@
         <v>69</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>36</v>
@@ -7957,16 +8010,16 @@
         <v>36</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X21" s="2" t="s">
         <v>111</v>
@@ -7975,18 +8028,18 @@
         <v>133</v>
       </c>
       <c r="AA21" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AC21" s="4" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>154</v>
@@ -8019,13 +8072,13 @@
         <v>117</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>36</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>36</v>
@@ -8037,39 +8090,39 @@
         <v>36</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AC22" s="4" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>22</v>
@@ -8099,13 +8152,13 @@
         <v>117</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>36</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P23" s="2" t="s">
         <v>36</v>
@@ -8117,16 +8170,16 @@
         <v>36</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X23" s="2" t="s">
         <v>111</v>
@@ -8135,18 +8188,18 @@
         <v>153</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AC23" s="4" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="24" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>83</v>
@@ -8176,51 +8229,51 @@
         <v>32</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P24" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="X24" s="2" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="Y24" s="1" t="s">
         <v>134</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="AC24" s="4" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="AD24" s="4" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>64</v>
@@ -8232,7 +8285,7 @@
         <v>3</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>63</v>
@@ -8253,7 +8306,7 @@
         <v>120</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>163</v>
@@ -8262,45 +8315,45 @@
         <v>36</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="S25" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="V25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="X25" s="2" t="s">
         <v>110</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AA25" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AC25" s="4" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="57" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>6</v>
@@ -8333,7 +8386,7 @@
         <v>117</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>36</v>
@@ -8348,45 +8401,45 @@
         <v>163</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="Y26" s="1" t="s">
         <v>135</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="AA26" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AB26" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AC26" s="4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="AD26" s="4" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="27" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>103</v>
@@ -8416,48 +8469,48 @@
         <v>33</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="U27" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="Y27" s="1" t="s">
         <v>136</v>
       </c>
       <c r="AA27" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AC27" s="4" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="28" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>5</v>
@@ -8490,7 +8543,7 @@
         <v>182</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>36</v>
@@ -8505,48 +8558,48 @@
         <v>163</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="U28" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W28" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="X28" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="Y28" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="X28" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="Y28" s="1" t="s">
-        <v>316</v>
-      </c>
       <c r="Z28" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="AA28" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AB28" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="AC28" s="4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="AD28" s="4" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="57" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>22</v>
@@ -8558,7 +8611,7 @@
         <v>24</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>77</v>
@@ -8576,60 +8629,60 @@
         <v>117</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>36</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P29" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U29" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="V29" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W29" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="X29" s="2" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Z29" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AA29" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="AB29" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="AC29" s="4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="AD29" s="4" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>22</v>
@@ -8641,10 +8694,10 @@
         <v>24</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>349</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>85</v>
@@ -8659,42 +8712,42 @@
         <v>117</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="T30" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="V30" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W30" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AA30" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AC30" s="4" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="31" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>22</v>
@@ -8724,51 +8777,51 @@
         <v>120</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O31" s="2" t="s">
         <v>36</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S31" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W31" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X31" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Y31" s="1" t="s">
         <v>141</v>
       </c>
       <c r="AA31" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AC31" s="4" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="32" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>22</v>
@@ -8798,13 +8851,13 @@
         <v>120</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>36</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Q32" s="2" t="s">
         <v>36</v>
@@ -8813,39 +8866,39 @@
         <v>36</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Y32" s="1" t="s">
         <v>142</v>
       </c>
       <c r="AA32" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AC32" s="4" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="33" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>22</v>
@@ -8875,51 +8928,51 @@
         <v>120</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O33" s="2" t="s">
         <v>36</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S33" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U33" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W33" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X33" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Y33" s="1" t="s">
         <v>137</v>
       </c>
       <c r="AA33" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AC33" s="4" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="34" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>22</v>
@@ -8949,28 +9002,28 @@
         <v>42</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O34" s="2" t="s">
         <v>36</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="T34" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="U34" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W34" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="X34" s="2" t="s">
         <v>112</v>
@@ -8979,21 +9032,21 @@
         <v>143</v>
       </c>
       <c r="AA34" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AC34" s="4" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="35" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>22</v>
@@ -9005,31 +9058,31 @@
         <v>30</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H35" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>208</v>
-      </c>
       <c r="J35" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="N35" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="K35" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="N35" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="O35" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P35" s="2" t="s">
         <v>162</v>
@@ -9038,48 +9091,48 @@
         <v>162</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="U35" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W35" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="X35" s="2" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Z35" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AA35" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AB35" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AC35" s="4" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="AD35" s="4" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="36" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>22</v>
@@ -9109,10 +9162,10 @@
         <v>170</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O36" s="2" t="s">
         <v>36</v>
@@ -9127,33 +9180,33 @@
         <v>36</v>
       </c>
       <c r="T36" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U36" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W36" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Y36" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="AA36" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AC36" s="4" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="37" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>175</v>
@@ -9186,7 +9239,7 @@
         <v>117</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>36</v>
@@ -9201,16 +9254,16 @@
         <v>163</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U37" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W37" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="X37" s="2" t="s">
         <v>173</v>
@@ -9219,21 +9272,21 @@
         <v>176</v>
       </c>
       <c r="AA37" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AC37" s="4" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="38" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>22</v>
@@ -9257,34 +9310,34 @@
         <v>68</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>117</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>163</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P38" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T38" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U38" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X38" s="2" t="s">
         <v>113</v>
@@ -9293,18 +9346,18 @@
         <v>138</v>
       </c>
       <c r="AA38" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AC38" s="4" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="39" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>12</v>
@@ -9337,48 +9390,48 @@
         <v>117</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N39" s="2" t="s">
         <v>163</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P39" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U39" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="V39" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W39" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X39" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="Y39" s="1" t="s">
         <v>139</v>
       </c>
       <c r="AA39" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AC39" s="4" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="40" spans="1:30" ht="57" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>13</v>
@@ -9411,45 +9464,45 @@
         <v>117</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P40" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="V40" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X40" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="Y40" s="1" t="s">
         <v>140</v>
       </c>
       <c r="AA40" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AC40" s="4" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="41" spans="1:30" ht="114" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>22</v>
@@ -9479,7 +9532,7 @@
         <v>181</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N41" s="2" t="s">
         <v>162</v>
@@ -9494,45 +9547,45 @@
         <v>163</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="U41" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="V41" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W41" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="X41" s="2" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="Y41" s="1" t="s">
         <v>183</v>
       </c>
       <c r="Z41" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="AA41" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AB41" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="AC41" s="4" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="AD41" s="4" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="42" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>14</v>
@@ -9565,10 +9618,10 @@
         <v>117</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="P42" s="2" t="s">
         <v>36</v>
@@ -9577,36 +9630,36 @@
         <v>163</v>
       </c>
       <c r="T42" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U42" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W42" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X42" s="2" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="Y42" s="1" t="s">
         <v>144</v>
       </c>
       <c r="AA42" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AC42" s="4" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="43" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>15</v>
@@ -9639,10 +9692,10 @@
         <v>117</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="P43" s="2" t="s">
         <v>36</v>
@@ -9651,36 +9704,36 @@
         <v>163</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="U43" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V43" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W43" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X43" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="Y43" s="1" t="s">
         <v>145</v>
       </c>
       <c r="AA43" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="AC43" s="4" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="44" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>16</v>
@@ -9713,10 +9766,10 @@
         <v>117</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="P44" s="2" t="s">
         <v>36</v>
@@ -9725,36 +9778,36 @@
         <v>163</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="U44" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V44" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W44" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X44" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="Y44" s="1" t="s">
         <v>146</v>
       </c>
       <c r="AA44" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AC44" s="4" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="45" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>17</v>
@@ -9787,10 +9840,10 @@
         <v>117</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="P45" s="2" t="s">
         <v>36</v>
@@ -9799,36 +9852,36 @@
         <v>163</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="U45" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V45" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W45" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X45" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="Y45" s="1" t="s">
         <v>147</v>
       </c>
       <c r="AA45" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="AC45" s="4" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="46" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>18</v>
@@ -9861,10 +9914,10 @@
         <v>117</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="P46" s="2" t="s">
         <v>36</v>
@@ -9873,39 +9926,39 @@
         <v>163</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="U46" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V46" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W46" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X46" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="Y46" s="1" t="s">
         <v>148</v>
       </c>
       <c r="AA46" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AC46" s="4" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="47" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>22</v>
@@ -9923,7 +9976,7 @@
         <v>72</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>68</v>
@@ -9935,42 +9988,42 @@
         <v>117</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P47" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T47" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U47" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="V47" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W47" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="Y47" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="AA47" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="AC47" s="4" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="48" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>22</v>
@@ -9979,7 +10032,7 @@
         <v>3</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>39</v>
@@ -10000,45 +10053,45 @@
         <v>69</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P48" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T48" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U48" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="V48" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W48" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X48" s="2" t="s">
         <v>113</v>
       </c>
       <c r="Y48" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="AA48" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="AC48" s="4" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="49" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>22</v>
@@ -10047,7 +10100,7 @@
         <v>3</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>24</v>
@@ -10068,45 +10121,45 @@
         <v>69</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P49" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T49" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="V49" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W49" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X49" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="Y49" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="AA49" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="AC49" s="4" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="50" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>22</v>
@@ -10115,7 +10168,7 @@
         <v>3</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>30</v>
@@ -10136,45 +10189,45 @@
         <v>69</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P50" s="2" t="s">
         <v>36</v>
       </c>
       <c r="T50" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U50" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="V50" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W50" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X50" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="Y50" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="AA50" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="AC50" s="4" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="51" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>22</v>
@@ -10204,13 +10257,13 @@
         <v>117</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N51" s="2" t="s">
         <v>163</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P51" s="2" t="s">
         <v>36</v>
@@ -10219,16 +10272,16 @@
         <v>163</v>
       </c>
       <c r="T51" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="U51" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V51" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W51" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X51" s="2" t="s">
         <v>113</v>
@@ -10237,18 +10290,18 @@
         <v>149</v>
       </c>
       <c r="AA51" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="AC51" s="4" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="52" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>19</v>
@@ -10281,13 +10334,13 @@
         <v>117</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>163</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P52" s="2" t="s">
         <v>36</v>
@@ -10296,36 +10349,36 @@
         <v>163</v>
       </c>
       <c r="T52" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="U52" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V52" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W52" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X52" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="Y52" s="1" t="s">
         <v>150</v>
       </c>
       <c r="AA52" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="AC52" s="4" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="53" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>20</v>
@@ -10358,13 +10411,13 @@
         <v>117</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N53" s="2" t="s">
         <v>163</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P53" s="2" t="s">
         <v>36</v>
@@ -10373,36 +10426,36 @@
         <v>163</v>
       </c>
       <c r="T53" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="U53" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V53" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W53" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="X53" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="Y53" s="1" t="s">
         <v>151</v>
       </c>
       <c r="AA53" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="AC53" s="4" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="54" spans="1:30" ht="171" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>121</v>
@@ -10435,7 +10488,7 @@
         <v>117</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N54" s="2" t="s">
         <v>36</v>
@@ -10450,48 +10503,48 @@
         <v>162</v>
       </c>
       <c r="T54" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="U54" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="V54" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W54" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="X54" s="2" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="Y54" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Z54" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="AA54" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AB54" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="AC54" s="4" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="AD54" s="5" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="55" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>22</v>
@@ -10506,7 +10559,7 @@
         <v>45</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>85</v>
@@ -10521,13 +10574,13 @@
         <v>117</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P55" s="2" t="s">
         <v>36</v>
@@ -10536,48 +10589,48 @@
         <v>162</v>
       </c>
       <c r="T55" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U55" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="V55" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W55" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="X55" s="2" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Y55" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="Z55" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="Z55" s="1" t="s">
-        <v>458</v>
-      </c>
       <c r="AA55" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="AB55" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="AC55" s="4" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="AD55" s="4" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>22</v>
@@ -10586,16 +10639,16 @@
         <v>3</v>
       </c>
       <c r="F56" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G56" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>42</v>
@@ -10604,54 +10657,54 @@
         <v>32</v>
       </c>
       <c r="L56" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q56" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R56" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T56" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="M56" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="N56" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="O56" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="P56" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q56" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R56" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T56" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="U56" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="W56" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Y56" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AA56" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AC56" s="4" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>22</v>
@@ -10660,16 +10713,16 @@
         <v>3</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>42</v>
@@ -10678,54 +10731,54 @@
         <v>32</v>
       </c>
       <c r="L57" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="O57" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="P57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T57" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="M57" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="N57" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="O57" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="P57" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q57" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R57" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T57" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="U57" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="W57" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Y57" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AA57" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AC57" s="4" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>22</v>
@@ -10734,7 +10787,7 @@
         <v>3</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>171</v>
@@ -10743,7 +10796,7 @@
         <v>73</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>42</v>
@@ -10752,54 +10805,54 @@
         <v>32</v>
       </c>
       <c r="L58" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="M58" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="N58" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="P58" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q58" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R58" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T58" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="M58" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="N58" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="O58" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="P58" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q58" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R58" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T58" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="U58" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="W58" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Y58" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AA58" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AC58" s="4" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>22</v>
@@ -10808,16 +10861,16 @@
         <v>3</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>42</v>
@@ -10826,54 +10879,54 @@
         <v>32</v>
       </c>
       <c r="L59" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="N59" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="O59" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="P59" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q59" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R59" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T59" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="M59" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="N59" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="O59" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="P59" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q59" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R59" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T59" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="U59" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="W59" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Y59" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AA59" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AC59" s="4" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>22</v>
@@ -10882,16 +10935,16 @@
         <v>3</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>42</v>
@@ -10900,54 +10953,54 @@
         <v>32</v>
       </c>
       <c r="L60" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="N60" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="O60" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="P60" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q60" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R60" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T60" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="M60" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="N60" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="O60" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="P60" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q60" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R60" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T60" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="U60" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="W60" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Y60" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AA60" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AC60" s="4" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>22</v>
@@ -10956,16 +11009,16 @@
         <v>3</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>42</v>
@@ -10974,54 +11027,54 @@
         <v>32</v>
       </c>
       <c r="L61" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="N61" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="O61" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="P61" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q61" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R61" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T61" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="M61" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="N61" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="O61" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="P61" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q61" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R61" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T61" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="U61" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="W61" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Y61" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AA61" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AC61" s="4" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="62" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>22</v>
@@ -11054,7 +11107,7 @@
         <v>37</v>
       </c>
       <c r="P62" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Q62" s="2" t="s">
         <v>36</v>
@@ -11063,16 +11116,16 @@
         <v>36</v>
       </c>
       <c r="T62" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="U62" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="V62" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="W62" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="X62" s="2" t="s">
         <v>167</v>
@@ -11081,18 +11134,18 @@
         <v>152</v>
       </c>
       <c r="AA62" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AC62" s="4" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="63" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>105</v>
@@ -11140,36 +11193,36 @@
         <v>36</v>
       </c>
       <c r="T63" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U63" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V63" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W63" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="Y63" s="1" t="s">
         <v>130</v>
       </c>
       <c r="AA63" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AC63" s="4" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A64" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>22</v>
@@ -11178,10 +11231,10 @@
         <v>3</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>77</v>
@@ -11199,7 +11252,7 @@
         <v>69</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N64" s="2" t="s">
         <v>36</v>
@@ -11214,28 +11267,28 @@
         <v>162</v>
       </c>
       <c r="T64" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="U64" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="V64" s="2" t="s">
         <v>32</v>
       </c>
       <c r="W64" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="X64" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="Y64" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="AA64" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="Y64" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="AA64" s="1" t="s">
-        <v>452</v>
-      </c>
       <c r="AC64" s="4" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update USB protocol specification document and add "CanChangeDeviceUsage" to ApplicationCommonSettings
</commit_message>
<xml_diff>
--- a/Documents/UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx
+++ b/Documents/UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="640">
   <si>
     <t>MessageId</t>
   </si>
@@ -5372,11 +5372,20 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>1.1.9000</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>public</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Developer</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1.1.9009</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Exvision
+(Basic)</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -6379,10 +6388,10 @@
   <dimension ref="A1:AD64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O15" sqref="O15"/>
+      <selection pane="bottomRight" activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -7590,13 +7599,13 @@
         <v>235</v>
       </c>
       <c r="U15" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="V15" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="V15" s="2" t="s">
-        <v>637</v>
-      </c>
       <c r="W15" s="2" t="s">
-        <v>319</v>
+        <v>639</v>
       </c>
       <c r="X15" s="2" t="s">
         <v>617</v>
@@ -7661,7 +7670,7 @@
         <v>32</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>189</v>
+        <v>637</v>
       </c>
       <c r="X16" s="2" t="s">
         <v>111</v>
@@ -11313,14 +11322,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x01010027AF63008C5B9348B1D80B486CE64D2D" ma:contentTypeVersion="4" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="104485263990d5adc83ab87317f77176">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns3="86e9103f-040a-4a6c-9c98-6d10a12a6690" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fee4f24d869e615bfcfb8b7a3dd1ece" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
@@ -11479,6 +11480,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FB82232-58B1-4A1D-8A4E-B5C95C1862BE}">
   <ds:schemaRefs>
@@ -11488,23 +11497,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153E850E-4F75-454A-AFBA-A711FED549FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="86e9103f-040a-4a6c-9c98-6d10a12a6690"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ED71AD8-9688-4B20-AAB5-757D07879363}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11521,4 +11513,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153E850E-4F75-454A-AFBA-A711FED549FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="86e9103f-040a-4a6c-9c98-6d10a12a6690"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implement functions related to EgsGestureHidReportMessageIds.ChangedSettingsByDevice
 * Added UpdateOnChangedSettingsByDevice() to EgsDeviceEgsGestureHidReport.
 * Added DevelopingFirmwareVersionString to VersionAndCultureInfo.t4 and ApplicationCommonSettings.
 * Fixed some bugs.
 * Still debugging.
</commit_message>
<xml_diff>
--- a/Documents/UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx
+++ b/Documents/UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx
@@ -5380,11 +5380,11 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>1.1.9009</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>Exvision
+    <t>1.1.9015</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Developer
 (Basic)</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -6391,7 +6391,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W15" sqref="W15"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -11322,6 +11322,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x01010027AF63008C5B9348B1D80B486CE64D2D" ma:contentTypeVersion="4" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="104485263990d5adc83ab87317f77176">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns3="86e9103f-040a-4a6c-9c98-6d10a12a6690" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fee4f24d869e615bfcfb8b7a3dd1ece" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
@@ -11480,14 +11488,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FB82232-58B1-4A1D-8A4E-B5C95C1862BE}">
   <ds:schemaRefs>
@@ -11497,6 +11497,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153E850E-4F75-454A-AFBA-A711FED549FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="86e9103f-040a-4a6c-9c98-6d10a12a6690"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ED71AD8-9688-4B20-AAB5-757D07879363}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11513,21 +11530,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153E850E-4F75-454A-AFBA-A711FED549FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="86e9103f-040a-4a6c-9c98-6d10a12a6690"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update resource strings excel files
</commit_message>
<xml_diff>
--- a/Documents/UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx
+++ b/Documents/UsbProtocol_EgsDeviceSettingsHidReport_HostAppSettings_PropertyList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -3314,47 +3314,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t>摄</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>像机</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-      </rPr>
-      <t>帧</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>每秒 (fps)</t>
-    </r>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <r>
       <t>120:120 fps
 100:100 fps
 0:自</t>
@@ -5153,86 +5112,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <r>
-      <t>0:相机</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>设备</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve">
-1:主</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>应</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>用程序 (更高精度)
-2:SDK用</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>户</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>自定</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="FangSong"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>义</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>解决方案</t>
-    </r>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>0:Remote Touch
 2:Motion Control
 1:Web Camera</t>
@@ -5386,6 +5265,126 @@
   <si>
     <t>Developer
 (Basic)</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+      </rPr>
+      <t>摄像头每秒帧数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve"> (fps)</t>
+    </r>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <r>
+      <t>0:手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="FangSong"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>势摄</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>像</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="FangSong"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>头</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">
+1:主</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="FangSong"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>应</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>用程序 (更高精度)
+2:SDK用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="FangSong"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>户</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>自定</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="FangSong"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>义</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>解决方案</t>
+    </r>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -6388,10 +6387,10 @@
   <dimension ref="A1:AD64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="AD17" sqref="AD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -6589,7 +6588,7 @@
         <v>359</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.15">
@@ -6737,7 +6736,7 @@
         <v>402</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.15">
@@ -6822,7 +6821,7 @@
         <v>268</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>442</v>
@@ -7113,7 +7112,7 @@
         <v>364</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.15">
@@ -7198,7 +7197,7 @@
         <v>269</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>432</v>
@@ -7258,7 +7257,7 @@
         <v>319</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Y11" s="1" t="s">
         <v>434</v>
@@ -7284,7 +7283,7 @@
         <v>269</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>81</v>
@@ -7347,7 +7346,7 @@
         <v>515</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="Y12" s="1" t="s">
         <v>131</v>
@@ -7362,7 +7361,7 @@
         <v>62</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="AD12" s="4" t="s">
         <v>420</v>
@@ -7373,7 +7372,7 @@
         <v>269</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
@@ -7436,7 +7435,7 @@
         <v>200</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Y13" s="1" t="s">
         <v>201</v>
@@ -7462,7 +7461,7 @@
         <v>269</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>82</v>
@@ -7525,7 +7524,7 @@
         <v>188</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Y14" s="1" t="s">
         <v>202</v>
@@ -7540,10 +7539,10 @@
         <v>422</v>
       </c>
       <c r="AC14" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="AD14" s="4" t="s">
         <v>599</v>
-      </c>
-      <c r="AD14" s="4" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
@@ -7551,7 +7550,7 @@
         <v>269</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>185</v>
@@ -7599,34 +7598,34 @@
         <v>235</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Y15" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="AA15" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="Z15" s="1" t="s">
+      <c r="AB15" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="AC15" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="AA15" s="1" t="s">
-        <v>626</v>
-      </c>
-      <c r="AB15" s="1" t="s">
+      <c r="AD15" s="4" t="s">
         <v>633</v>
-      </c>
-      <c r="AC15" s="5" t="s">
-        <v>634</v>
-      </c>
-      <c r="AD15" s="4" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.15">
@@ -7670,7 +7669,7 @@
         <v>32</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="X16" s="2" t="s">
         <v>111</v>
@@ -7682,7 +7681,7 @@
         <v>367</v>
       </c>
       <c r="AC16" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="71.25" x14ac:dyDescent="0.15">
@@ -7690,7 +7689,7 @@
         <v>269</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>533</v>
@@ -7732,19 +7731,19 @@
         <v>534</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="AA17" s="1" t="s">
         <v>535</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>631</v>
+        <v>639</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -7850,7 +7849,7 @@
         <v>69</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>36</v>
@@ -7912,7 +7911,7 @@
         <v>85</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>32</v>
@@ -7951,7 +7950,7 @@
         <v>517</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="Y20" s="1" t="s">
         <v>546</v>
@@ -8040,7 +8039,7 @@
         <v>369</v>
       </c>
       <c r="AC21" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
@@ -8208,7 +8207,7 @@
         <v>269</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>83</v>
@@ -8256,7 +8255,7 @@
         <v>518</v>
       </c>
       <c r="X24" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Y24" s="1" t="s">
         <v>134</v>
@@ -8362,7 +8361,7 @@
         <v>269</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>6</v>
@@ -8422,7 +8421,7 @@
         <v>317</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="Y26" s="1" t="s">
         <v>135</v>
@@ -8519,7 +8518,7 @@
         <v>269</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>5</v>
@@ -8579,7 +8578,7 @@
         <v>314</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Y28" s="1" t="s">
         <v>315</v>
@@ -8593,11 +8592,11 @@
       <c r="AB28" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="AC28" s="4" t="s">
+      <c r="AC28" s="6" t="s">
+        <v>638</v>
+      </c>
+      <c r="AD28" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="AD28" s="4" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="57" x14ac:dyDescent="0.15">
@@ -8605,7 +8604,7 @@
         <v>269</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>352</v>
@@ -8662,7 +8661,7 @@
         <v>187</v>
       </c>
       <c r="X29" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="Y29" s="1" t="s">
         <v>354</v>
@@ -8680,7 +8679,7 @@
         <v>427</v>
       </c>
       <c r="AD29" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.15">
@@ -8896,7 +8895,7 @@
         <v>377</v>
       </c>
       <c r="AC32" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="33" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -9044,7 +9043,7 @@
         <v>379</v>
       </c>
       <c r="AC34" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="35" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
@@ -9112,7 +9111,7 @@
         <v>342</v>
       </c>
       <c r="X35" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="Y35" s="1" t="s">
         <v>212</v>
@@ -9127,7 +9126,7 @@
         <v>341</v>
       </c>
       <c r="AC35" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="AD35" s="4" t="s">
         <v>430</v>
@@ -9207,7 +9206,7 @@
         <v>381</v>
       </c>
       <c r="AC36" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="37" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -9284,7 +9283,7 @@
         <v>382</v>
       </c>
       <c r="AC37" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="38" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -9358,7 +9357,7 @@
         <v>383</v>
       </c>
       <c r="AC38" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="39" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -9432,7 +9431,7 @@
         <v>384</v>
       </c>
       <c r="AC39" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="40" spans="1:30" ht="57" x14ac:dyDescent="0.15">
@@ -9500,7 +9499,7 @@
         <v>385</v>
       </c>
       <c r="AC40" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="41" spans="1:30" ht="114" x14ac:dyDescent="0.15">
@@ -9508,10 +9507,10 @@
         <v>269</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>22</v>
@@ -9568,7 +9567,7 @@
         <v>188</v>
       </c>
       <c r="X41" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Y41" s="1" t="s">
         <v>183</v>
@@ -9583,10 +9582,10 @@
         <v>423</v>
       </c>
       <c r="AC41" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AD41" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="42" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -9651,7 +9650,7 @@
         <v>520</v>
       </c>
       <c r="X42" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="Y42" s="1" t="s">
         <v>144</v>
@@ -9660,7 +9659,7 @@
         <v>387</v>
       </c>
       <c r="AC42" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="43" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -9734,7 +9733,7 @@
         <v>489</v>
       </c>
       <c r="AC43" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="44" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
@@ -9808,7 +9807,7 @@
         <v>388</v>
       </c>
       <c r="AC44" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="45" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -9882,7 +9881,7 @@
         <v>490</v>
       </c>
       <c r="AC45" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="46" spans="1:30" ht="42.75" x14ac:dyDescent="0.15">
@@ -9956,7 +9955,7 @@
         <v>389</v>
       </c>
       <c r="AC46" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="47" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -10021,7 +10020,7 @@
         <v>471</v>
       </c>
       <c r="AC47" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="48" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -10089,7 +10088,7 @@
         <v>491</v>
       </c>
       <c r="AC48" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="49" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -10157,7 +10156,7 @@
         <v>492</v>
       </c>
       <c r="AC49" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="50" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -10225,7 +10224,7 @@
         <v>493</v>
       </c>
       <c r="AC50" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="51" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -10379,7 +10378,7 @@
         <v>495</v>
       </c>
       <c r="AC52" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="53" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -10456,7 +10455,7 @@
         <v>496</v>
       </c>
       <c r="AC53" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="54" spans="1:30" ht="171" x14ac:dyDescent="0.15">
@@ -10464,7 +10463,7 @@
         <v>271</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>121</v>
@@ -10524,7 +10523,7 @@
         <v>186</v>
       </c>
       <c r="X54" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Y54" s="1" t="s">
         <v>313</v>
@@ -10539,10 +10538,10 @@
         <v>439</v>
       </c>
       <c r="AC54" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="AD54" s="5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="55" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -10550,7 +10549,7 @@
         <v>269</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>452</v>
@@ -10610,7 +10609,7 @@
         <v>186</v>
       </c>
       <c r="X55" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="Y55" s="1" t="s">
         <v>454</v>
@@ -10625,7 +10624,7 @@
         <v>455</v>
       </c>
       <c r="AC55" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AD55" s="4" t="s">
         <v>467</v>
@@ -10702,7 +10701,7 @@
         <v>391</v>
       </c>
       <c r="AC56" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.15">
@@ -10776,7 +10775,7 @@
         <v>392</v>
       </c>
       <c r="AC57" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.15">
@@ -10924,7 +10923,7 @@
         <v>394</v>
       </c>
       <c r="AC59" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.15">
@@ -10998,7 +10997,7 @@
         <v>395</v>
       </c>
       <c r="AC60" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.15">
@@ -11146,7 +11145,7 @@
         <v>397</v>
       </c>
       <c r="AC62" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="63" spans="1:30" ht="28.5" x14ac:dyDescent="0.15">
@@ -11220,7 +11219,7 @@
         <v>398</v>
       </c>
       <c r="AC63" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.15">
@@ -11297,7 +11296,7 @@
         <v>450</v>
       </c>
       <c r="AC64" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
   </sheetData>
@@ -11322,14 +11321,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x01010027AF63008C5B9348B1D80B486CE64D2D" ma:contentTypeVersion="4" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="104485263990d5adc83ab87317f77176">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns3="86e9103f-040a-4a6c-9c98-6d10a12a6690" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fee4f24d869e615bfcfb8b7a3dd1ece" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
@@ -11488,6 +11479,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FB82232-58B1-4A1D-8A4E-B5C95C1862BE}">
   <ds:schemaRefs>
@@ -11497,23 +11496,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153E850E-4F75-454A-AFBA-A711FED549FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="86e9103f-040a-4a6c-9c98-6d10a12a6690"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ED71AD8-9688-4B20-AAB5-757D07879363}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11530,4 +11512,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153E850E-4F75-454A-AFBA-A711FED549FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="86e9103f-040a-4a6c-9c98-6d10a12a6690"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>